<commit_message>
updated sales and stock share handling for usrr and nems
</commit_message>
<xml_diff>
--- a/data-raw/model-runs/USREP-ReEDS additional Reporting Variables 8.13.xlsx
+++ b/data-raw/model-runs/USREP-ReEDS additional Reporting Variables 8.13.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\BTR\data-raw\model-runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34529C2D-FD65-4ACD-B94D-6CE61049A43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DCFF6C-A464-4F3C-AB60-EF5E214BC6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BA981C3-0E63-4417-BD30-5140A226A9C3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>USA</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Energy Service|Transportation|Passenger|PHEV|Stock Share</t>
+  </si>
+  <si>
+    <t>Energy Service|Transportation|Freight|BEV|Sales Share</t>
+  </si>
+  <si>
+    <t>Energy Service|Transportation|Freight|ICE|Sales Share</t>
   </si>
 </sst>
 </file>
@@ -451,7 +457,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,8 +662,69 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>

</xml_diff>